<commit_message>
Modified Code Fetched data from excel
</commit_message>
<xml_diff>
--- a/employees_data.xlsx
+++ b/employees_data.xlsx
@@ -1,41 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tushar ERP MERN\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264"/>
+  </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Employment Type</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Check-In</t>
+  </si>
+  <si>
+    <t>Check-Out</t>
+  </si>
+  <si>
+    <t>Work Type</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +86,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,145 +418,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>employeeId</v>
-      </c>
-      <c r="B1" t="str">
-        <v>name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>role</v>
-      </c>
-      <c r="D1" t="str">
-        <v>employmentType</v>
-      </c>
-      <c r="E1" t="str">
-        <v>status</v>
-      </c>
-      <c r="F1" t="str">
-        <v>checkIn</v>
-      </c>
-      <c r="G1" t="str">
-        <v>checkOut</v>
-      </c>
-      <c r="H1" t="str">
-        <v>workType</v>
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2">
-        <v>123</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Tejas Doe</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Manager</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Full-Time</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Active</v>
-      </c>
-      <c r="F2" t="str">
-        <v>09:00 AM</v>
-      </c>
-      <c r="G2" t="str">
-        <v>05:00 PM</v>
-      </c>
-      <c r="H2" t="str">
-        <v>Onsite</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>345</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Tejas Doe</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Manager</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Full-Time</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Active</v>
-      </c>
-      <c r="F3" t="str">
-        <v>09:00 AM</v>
-      </c>
-      <c r="G3" t="str">
-        <v>05:00 PM</v>
-      </c>
-      <c r="H3" t="str">
-        <v>Onsite</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>1234</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Tejas Doe</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Manager</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Full-Time</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Active</v>
-      </c>
-      <c r="F4" t="str">
-        <v>09:00 AM</v>
-      </c>
-      <c r="G4" t="str">
-        <v>05:00 PM</v>
-      </c>
-      <c r="H4" t="str">
-        <v>Onsite</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>344343</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Bisen Tejas</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Manager</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Full-Time</v>
-      </c>
-      <c r="E5" t="str">
-        <v>Active</v>
-      </c>
-      <c r="F5" t="str">
-        <v>09:00 AM</v>
-      </c>
-      <c r="G5" t="str">
-        <v>05:00 PM</v>
-      </c>
-      <c r="H5" t="str">
-        <v>Onsite</v>
-      </c>
-    </row>
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError sqref="A1:H1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>